<commit_message>
Entrega Final – laboratorio 5
</commit_message>
<xml_diff>
--- a/Docs/ISIS1225 - TablasDatos-Lab4-5.xlsx
+++ b/Docs/ISIS1225 - TablasDatos-Lab4-5.xlsx
@@ -16,14 +16,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataSignature="AMtx7mjt/6Jd/S/kqdUYrcVHpaKXNi/0nw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataSignature="AMtx7mibBTDEBstp/rLNLsM0x8TETex+hg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>Porcentaje de la muestra [pct]</t>
   </si>
@@ -63,7 +63,10 @@
     <t>Merge Sort [ms]</t>
   </si>
   <si>
-    <t>Computadora 3</t>
+    <t>34.081.75</t>
+  </si>
+  <si>
+    <t>56.648.33</t>
   </si>
   <si>
     <t>Tamaño de la muestra (LINKED_LIST)</t>
@@ -71,84 +74,12 @@
   <si>
     <t>&gt;10 min</t>
   </si>
-  <si>
-    <t>Computadora 1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="dax-regular"/>
-        <b/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Dax-Regular"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>amaño de la muestra (ARRAY_LIST)</t>
-    </r>
-  </si>
-  <si>
-    <t>Computadora 2</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="dax-regular"/>
-        <b/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Dax-Regular"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>amaño de la muestra (ARRAY_LIST)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="dax-regular"/>
-        <b/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Dax-Regular"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>amaño de la muestra (ARRAY_LIST)</t>
-    </r>
-  </si>
-  <si>
-    <t>34.081.75</t>
-  </si>
-  <si>
-    <t>56.648.33</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -173,17 +104,11 @@
       <name val="Dax-regular"/>
     </font>
     <font>
+      <sz val="11.0"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -203,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -220,22 +145,16 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
   </cellXfs>
@@ -281,43 +200,13 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="8">
+  <tableStyles count="2">
     <tableStyle count="3" pivot="0" name="Datos Lab4-5-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="3" pivot="0" name="Datos Lab4-5-style 2">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
-    </tableStyle>
-    <tableStyle count="3" pivot="0" name="Datos Lab4-5-style 3">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
-    </tableStyle>
-    <tableStyle count="3" pivot="0" name="Datos Lab4-5-style 4">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
-    </tableStyle>
-    <tableStyle count="3" pivot="0" name="Datos Lab4-5-style 5">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
-    </tableStyle>
-    <tableStyle count="3" pivot="0" name="Datos Lab4-5-style 6">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
-    </tableStyle>
-    <tableStyle count="3" pivot="0" name="Datos Lab4-5-style 7">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
-    </tableStyle>
-    <tableStyle count="3" pivot="0" name="Datos Lab4-5-style 8">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -404,19 +293,17 @@
             </c:spPr>
           </c:marker>
           <c:trendline>
-            <c:name/>
+            <c:name>Expon. (Insertion Sort [ms])</c:name>
             <c:spPr>
               <a:ln w="19050">
                 <a:solidFill>
-                  <a:srgbClr val="FF9900">
-                    <a:alpha val="80000"/>
-                  </a:srgbClr>
+                  <a:srgbClr val="FF9900"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="exp"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -466,7 +353,7 @@
             </c:spPr>
             <c:trendlineType val="exp"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -493,7 +380,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="7"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
@@ -506,11 +393,63 @@
             </c:spPr>
           </c:marker>
           <c:trendline>
+            <c:name>Linear (Shell Sort [ms])</c:name>
+            <c:spPr>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:srgbClr val="FFC000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Datos Lab4-5'!$A$2:$A$9</c:f>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Datos Lab4-5'!$E$2:$E$9</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Quick Sort [ms]</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
             <c:name/>
             <c:spPr>
               <a:ln w="19050">
                 <a:solidFill>
-                  <a:srgbClr val="FFFF00"/>
+                  <a:srgbClr val="000000">
+                    <a:alpha val="0"/>
+                  </a:srgbClr>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
@@ -525,7 +464,57 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$E$2:$E$9</c:f>
+              <c:f>'Datos Lab4-5'!$F$2:$F$9</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Merge Sort [ms]</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:name/>
+            <c:spPr>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Datos Lab4-5'!$A$2:$A$9</c:f>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Datos Lab4-5'!$G$2:$G$9</c:f>
               <c:numCache/>
             </c:numRef>
           </c:yVal>
@@ -538,11 +527,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="779566307"/>
-        <c:axId val="218479538"/>
+        <c:axId val="1972814112"/>
+        <c:axId val="1814570809"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="779566307"/>
+        <c:axId val="1972814112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -606,10 +595,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218479538"/>
+        <c:crossAx val="1814570809"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218479538"/>
+        <c:axId val="1814570809"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -673,7 +662,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="779566307"/>
+        <c:crossAx val="1972814112"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -777,7 +766,7 @@
             </c:spPr>
           </c:marker>
           <c:trendline>
-            <c:name/>
+            <c:name>Expon. (Insertion Sort [ms])</c:name>
             <c:spPr>
               <a:ln w="19050">
                 <a:solidFill>
@@ -787,7 +776,7 @@
             </c:spPr>
             <c:trendlineType val="exp"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -837,7 +826,7 @@
             </c:spPr>
             <c:trendlineType val="exp"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -887,7 +876,7 @@
             </c:spPr>
             <c:trendlineType val="exp"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -901,6 +890,108 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Quick Sort [ms]</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:name/>
+            <c:spPr>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:srgbClr val="0000FF">
+                    <a:alpha val="40000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Datos Lab4-5'!$A$13:$A$20</c:f>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Datos Lab4-5'!$F$13:$F$20</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Merge Sort [ms]</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:name/>
+            <c:spPr>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Datos Lab4-5'!$A$13:$A$20</c:f>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Datos Lab4-5'!$G$13:$G$20</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -909,11 +1000,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="810650006"/>
-        <c:axId val="1733399182"/>
+        <c:axId val="523765968"/>
+        <c:axId val="911216512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="810650006"/>
+        <c:axId val="523765968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -977,10 +1068,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1733399182"/>
+        <c:crossAx val="911216512"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1733399182"/>
+        <c:axId val="911216512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1044,7 +1135,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="810650006"/>
+        <c:crossAx val="523765968"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1132,17 +1223,17 @@
             </c:spPr>
           </c:marker>
           <c:trendline>
-            <c:name/>
+            <c:name>Linear (Insertion Sort [ms])</c:name>
             <c:spPr>
               <a:ln w="19050">
                 <a:solidFill>
-                  <a:srgbClr val="4A86E8"/>
+                  <a:srgbClr val="4472C4"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="exp"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1164,11 +1255,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2032833800"/>
-        <c:axId val="1517921404"/>
+        <c:axId val="347399572"/>
+        <c:axId val="1876292611"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2032833800"/>
+        <c:axId val="347399572"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1232,10 +1323,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1517921404"/>
+        <c:crossAx val="1876292611"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1517921404"/>
+        <c:axId val="1876292611"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1299,7 +1390,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2032833800"/>
+        <c:crossAx val="347399572"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1387,17 +1478,17 @@
             </c:spPr>
           </c:marker>
           <c:trendline>
-            <c:name/>
+            <c:name>Linear (Selection Sort [ms])</c:name>
             <c:spPr>
               <a:ln w="19050">
                 <a:solidFill>
-                  <a:srgbClr val="4A86E8"/>
+                  <a:srgbClr val="4472C4"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="exp"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1419,11 +1510,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="974743524"/>
-        <c:axId val="1643268555"/>
+        <c:axId val="129487392"/>
+        <c:axId val="1839708438"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="974743524"/>
+        <c:axId val="129487392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1487,10 +1578,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1643268555"/>
+        <c:crossAx val="1839708438"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1643268555"/>
+        <c:axId val="1839708438"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1554,7 +1645,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="974743524"/>
+        <c:crossAx val="129487392"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1642,17 +1733,17 @@
             </c:spPr>
           </c:marker>
           <c:trendline>
-            <c:name/>
+            <c:name>Linear (Shell Sort [ms])</c:name>
             <c:spPr>
               <a:ln w="19050">
                 <a:solidFill>
-                  <a:srgbClr val="4A86E8"/>
+                  <a:srgbClr val="4472C4"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="exp"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1674,11 +1765,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="605066013"/>
-        <c:axId val="664285559"/>
+        <c:axId val="1067056207"/>
+        <c:axId val="442217356"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="605066013"/>
+        <c:axId val="1067056207"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1742,10 +1833,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="664285559"/>
+        <c:crossAx val="442217356"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="664285559"/>
+        <c:axId val="442217356"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1809,7 +1900,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="605066013"/>
+        <c:crossAx val="1067056207"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1879,6 +1970,56 @@
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Quick Sort [ms]</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:name>Linear (Quick Sort [ms])</c:name>
+            <c:spPr>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:srgbClr val="4472C4"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Datos Lab4-5'!$A$2:$A$9</c:f>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Datos Lab4-5'!$F$2:$F$9</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1887,11 +2028,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1344524130"/>
-        <c:axId val="719849660"/>
+        <c:axId val="418530288"/>
+        <c:axId val="1217587208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1344524130"/>
+        <c:axId val="418530288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1955,22 +2096,74 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="719849660"/>
+        <c:crossAx val="1217587208"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="719849660"/>
+        <c:axId val="1217587208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="1" i="0" sz="1000">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" i="0" sz="1000">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Tiempo de Ejecución [ms]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
+          <a:ln/>
         </c:spPr>
-        <c:crossAx val="1344524130"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="418530288"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2040,6 +2233,56 @@
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Merge Sort [ms]</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:name/>
+            <c:spPr>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:srgbClr val="4472C4"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Datos Lab4-5'!$A$2:$A$9</c:f>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Datos Lab4-5'!$G$2:$G$9</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2048,11 +2291,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1371015795"/>
-        <c:axId val="1552145749"/>
+        <c:axId val="923267007"/>
+        <c:axId val="1162662515"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1371015795"/>
+        <c:axId val="923267007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2116,22 +2359,74 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1552145749"/>
+        <c:crossAx val="1162662515"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1552145749"/>
+        <c:axId val="1162662515"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="1" i="0" sz="1000">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" i="0" sz="1000">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Tiempo de Ejecución [ms]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
+          <a:ln/>
         </c:spPr>
-        <c:crossAx val="1371015795"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="923267007"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2231,7 +2526,7 @@
     <xdr:ext cx="8610600" cy="6276975"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1374329456" name="Chart 1" title="Gráfico"/>
+        <xdr:cNvPr id="163341320" name="Chart 1" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2256,7 +2551,7 @@
     <xdr:ext cx="8610600" cy="6276975"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="245827546" name="Chart 2" title="Gráfico"/>
+        <xdr:cNvPr id="895442876" name="Chart 2" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2281,7 +2576,7 @@
     <xdr:ext cx="8610600" cy="6276975"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1256938528" name="Chart 3" title="Gráfico"/>
+        <xdr:cNvPr id="1790603115" name="Chart 3" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2306,7 +2601,7 @@
     <xdr:ext cx="8610600" cy="6276975"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1079208038" name="Chart 4" title="Gráfico"/>
+        <xdr:cNvPr id="58030456" name="Chart 4" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2331,7 +2626,7 @@
     <xdr:ext cx="8610600" cy="6276975"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="641015346" name="Chart 5" title="Gráfico"/>
+        <xdr:cNvPr id="992548804" name="Chart 5" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2356,7 +2651,7 @@
     <xdr:ext cx="8610600" cy="6276975"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1065160776" name="Chart 6"/>
+        <xdr:cNvPr id="544795817" name="Chart 6" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2381,7 +2676,7 @@
     <xdr:ext cx="8610600" cy="6276975"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="398981000" name="Chart 7"/>
+        <xdr:cNvPr id="1617103997" name="Chart 7" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2400,17 +2695,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G9" displayName="Table_1" id="1">
-  <tableColumns count="7">
-    <tableColumn name="Porcentaje de la muestra [pct]" id="1"/>
-    <tableColumn name="Tamaño de la muestra (ARRAY_LIST)" id="2"/>
-    <tableColumn name="Insertion Sort [ms]" id="3"/>
-    <tableColumn name="Selection Sort [ms]" id="4"/>
-    <tableColumn name="Shell Sort [ms]" id="5"/>
-    <tableColumn name="Quick Sort [ms]" id="6"/>
-    <tableColumn name="Merge Sort [ms]" id="7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A1:H9" displayName="Table_1" id="1">
+  <tableColumns count="8">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+    <tableColumn name="Column6" id="6"/>
+    <tableColumn name="Column7" id="7"/>
+    <tableColumn name="Column8" id="8"/>
   </tableColumns>
   <tableStyleInfo name="Datos Lab4-5-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
+    </ext>
+  </extLst>
 </table>
 </file>
 
@@ -2426,106 +2727,6 @@
     <tableColumn name="Merge Sort [ms]" id="7"/>
   </tableColumns>
   <tableStyleInfo name="Datos Lab4-5-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A26:G34" displayName="Table_3" id="3">
-  <tableColumns count="7">
-    <tableColumn name="Porcentaje de la muestra [pct]" id="1"/>
-    <tableColumn name="Tamaño de la muestra (ARRAY_LIST)" id="2"/>
-    <tableColumn name="Insertion Sort [ms]" id="3"/>
-    <tableColumn name="Selection Sort [ms]" id="4"/>
-    <tableColumn name="Shell Sort [ms]" id="5"/>
-    <tableColumn name="Quick Sort [ms]" id="6"/>
-    <tableColumn name="Merge Sort [ms]" id="7"/>
-  </tableColumns>
-  <tableStyleInfo name="Datos Lab4-5-style 3" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A37:G45" displayName="Table_4" id="4">
-  <tableColumns count="7">
-    <tableColumn name="Porcentaje de la muestra [pct]" id="1"/>
-    <tableColumn name="Tamaño de la muestra (LINKED_LIST)" id="2"/>
-    <tableColumn name="Insertion Sort [ms]" id="3"/>
-    <tableColumn name="Selection Sort [ms]" id="4"/>
-    <tableColumn name="Shell Sort [ms]" id="5"/>
-    <tableColumn name="Quick Sort [ms]" id="6"/>
-    <tableColumn name="Merge Sort [ms]" id="7"/>
-  </tableColumns>
-  <tableStyleInfo name="Datos Lab4-5-style 4" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A51:G59" displayName="Table_5" id="5">
-  <tableColumns count="7">
-    <tableColumn name="Porcentaje de la muestra [pct]" id="1"/>
-    <tableColumn name="Tamaño de la muestra (ARRAY_LIST)" id="2"/>
-    <tableColumn name="Insertion Sort [ms]" id="3"/>
-    <tableColumn name="Selection Sort [ms]" id="4"/>
-    <tableColumn name="Shell Sort [ms]" id="5"/>
-    <tableColumn name="Quick Sort [ms]" id="6"/>
-    <tableColumn name="Merge Sort [ms]" id="7"/>
-  </tableColumns>
-  <tableStyleInfo name="Datos Lab4-5-style 5" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A62:G70" displayName="Table_6" id="6">
-  <tableColumns count="7">
-    <tableColumn name="Porcentaje de la muestra [pct]" id="1"/>
-    <tableColumn name="Tamaño de la muestra (LINKED_LIST)" id="2"/>
-    <tableColumn name="Insertion Sort [ms]" id="3"/>
-    <tableColumn name="Selection Sort [ms]" id="4"/>
-    <tableColumn name="Shell Sort [ms]" id="5"/>
-    <tableColumn name="Quick Sort [ms]" id="6"/>
-    <tableColumn name="Merge Sort [ms]" id="7"/>
-  </tableColumns>
-  <tableStyleInfo name="Datos Lab4-5-style 6" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A75:G83" displayName="Table_7" id="7">
-  <tableColumns count="7">
-    <tableColumn name="Column1" id="1"/>
-    <tableColumn name="Column2" id="2"/>
-    <tableColumn name="Column3" id="3"/>
-    <tableColumn name="Column4" id="4"/>
-    <tableColumn name="Column5" id="5"/>
-    <tableColumn name="Column6" id="6"/>
-    <tableColumn name="Column7" id="7"/>
-  </tableColumns>
-  <tableStyleInfo name="Datos Lab4-5-style 7" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
-    </ext>
-  </extLst>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A86:G94" displayName="Table_8" id="8">
-  <tableColumns count="7">
-    <tableColumn name="Column1" id="1"/>
-    <tableColumn name="Column2" id="2"/>
-    <tableColumn name="Column3" id="3"/>
-    <tableColumn name="Column4" id="4"/>
-    <tableColumn name="Column5" id="5"/>
-    <tableColumn name="Column6" id="6"/>
-    <tableColumn name="Column7" id="7"/>
-  </tableColumns>
-  <tableStyleInfo name="Datos Lab4-5-style 8" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
-    </ext>
-  </extLst>
 </table>
 </file>
 
@@ -2764,7 +2965,7 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -2792,16 +2993,21 @@
         <v>49.0</v>
       </c>
       <c r="C2" s="5">
-        <v>11.29</v>
+        <v>7.45</v>
       </c>
       <c r="D2" s="5">
-        <v>16.71</v>
+        <v>5.93</v>
       </c>
       <c r="E2" s="5">
-        <v>6.63</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+        <v>3.17</v>
+      </c>
+      <c r="F2" s="5">
+        <v>4.32</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1.36</v>
+      </c>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3">
@@ -2811,16 +3017,21 @@
         <v>245.0</v>
       </c>
       <c r="C3" s="5">
-        <v>134.72</v>
+        <v>215.79</v>
       </c>
       <c r="D3" s="5">
-        <v>271.48</v>
+        <v>104.37</v>
       </c>
       <c r="E3" s="5">
-        <v>77.05</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+        <v>31.94</v>
+      </c>
+      <c r="F3" s="5">
+        <v>19.02</v>
+      </c>
+      <c r="G3" s="6">
+        <v>14.79</v>
+      </c>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3">
@@ -2829,20 +3040,22 @@
       <c r="B4" s="4">
         <v>490.0</v>
       </c>
-      <c r="C4" s="5">
-        <v>480.21</v>
+      <c r="C4" s="7">
+        <v>456.36</v>
       </c>
       <c r="D4" s="5">
-        <v>926.24</v>
+        <v>1042.84</v>
       </c>
       <c r="E4" s="5">
-        <v>217.73</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="I4" s="7" t="s">
-        <v>7</v>
-      </c>
+        <v>88.77</v>
+      </c>
+      <c r="F4" s="5">
+        <v>43.09</v>
+      </c>
+      <c r="G4" s="6">
+        <v>36.75</v>
+      </c>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="3">
@@ -2852,16 +3065,21 @@
         <v>980.0</v>
       </c>
       <c r="C5" s="5">
-        <v>1901.95</v>
+        <v>1234.56</v>
       </c>
       <c r="D5" s="5">
-        <v>3471.01</v>
+        <v>3093.55</v>
       </c>
       <c r="E5" s="5">
-        <v>534.57</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+        <v>199.55</v>
+      </c>
+      <c r="F5" s="5">
+        <v>85.58</v>
+      </c>
+      <c r="G5" s="6">
+        <v>69.51</v>
+      </c>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3">
@@ -2871,16 +3089,21 @@
         <v>1470.0</v>
       </c>
       <c r="C6" s="5">
-        <v>4453.74</v>
+        <v>3843.64</v>
       </c>
       <c r="D6" s="5">
-        <v>7945.44</v>
+        <v>5204.79</v>
       </c>
       <c r="E6" s="5">
-        <v>910.21</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+        <v>353.86</v>
+      </c>
+      <c r="F6" s="5">
+        <v>198.24</v>
+      </c>
+      <c r="G6" s="6">
+        <v>114.38</v>
+      </c>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3">
@@ -2890,16 +3113,21 @@
         <v>2451.0</v>
       </c>
       <c r="C7" s="5">
-        <v>12329.42</v>
+        <v>8679.57</v>
       </c>
       <c r="D7" s="5">
-        <v>21427.23</v>
+        <v>13126.63</v>
       </c>
       <c r="E7" s="5">
-        <v>1658.79</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+        <v>634.78</v>
+      </c>
+      <c r="F7" s="5">
+        <v>262.27</v>
+      </c>
+      <c r="G7" s="6">
+        <v>202.58</v>
+      </c>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="3">
@@ -2909,16 +3137,21 @@
         <v>3922.0</v>
       </c>
       <c r="C8" s="5">
-        <v>32511.23</v>
+        <v>21591.45</v>
       </c>
       <c r="D8" s="5">
-        <v>60648.2</v>
+        <v>34365.41</v>
       </c>
       <c r="E8" s="5">
-        <v>3052.8</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+        <v>1541.28</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1008.98</v>
+      </c>
+      <c r="G8" s="6">
+        <v>611.99</v>
+      </c>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3">
@@ -2927,17 +3160,22 @@
       <c r="B9" s="4">
         <v>4903.0</v>
       </c>
-      <c r="C9" s="5">
-        <v>49950.18</v>
-      </c>
-      <c r="D9" s="5">
-        <v>88782.28</v>
+      <c r="C9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E9" s="5">
-        <v>4514.55</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+        <v>2228.14</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1365.33</v>
+      </c>
+      <c r="G9" s="6">
+        <v>526.3</v>
+      </c>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="8"/>
@@ -2956,7 +3194,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>2</v>
@@ -3001,16 +3239,20 @@
         <v>49.0</v>
       </c>
       <c r="C13" s="5">
-        <v>12.95</v>
+        <v>13.77</v>
       </c>
       <c r="D13" s="5">
-        <v>30.51</v>
+        <v>24.95</v>
       </c>
       <c r="E13" s="5">
-        <v>12.82</v>
-      </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+        <v>17.78</v>
+      </c>
+      <c r="F13" s="5">
+        <v>7.65</v>
+      </c>
+      <c r="G13" s="5">
+        <v>4.13</v>
+      </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="3">
@@ -3020,16 +3262,20 @@
         <v>245.0</v>
       </c>
       <c r="C14" s="5">
-        <v>799.27</v>
+        <v>1299.6</v>
       </c>
       <c r="D14" s="5">
-        <v>827.65</v>
+        <v>1646.97</v>
       </c>
       <c r="E14" s="5">
-        <v>180.69</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+        <v>163.37</v>
+      </c>
+      <c r="F14" s="5">
+        <v>117.61</v>
+      </c>
+      <c r="G14" s="5">
+        <v>31.21</v>
+      </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3">
@@ -3038,17 +3284,21 @@
       <c r="B15" s="4">
         <v>490.0</v>
       </c>
-      <c r="C15" s="4">
-        <v>6502.13</v>
+      <c r="C15" s="9">
+        <v>8982.75</v>
       </c>
       <c r="D15" s="4">
-        <v>6597.85</v>
+        <v>12987.7</v>
       </c>
       <c r="E15" s="4">
-        <v>642.96</v>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+        <v>570.53</v>
+      </c>
+      <c r="F15" s="4">
+        <v>525.07</v>
+      </c>
+      <c r="G15" s="4">
+        <v>207.3</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3">
@@ -3057,17 +3307,21 @@
       <c r="B16" s="4">
         <v>980.0</v>
       </c>
-      <c r="C16" s="4">
-        <v>51349.88</v>
+      <c r="C16" s="9">
+        <v>98123.87</v>
       </c>
       <c r="D16" s="4">
-        <v>57891.29</v>
+        <v>79528.31</v>
       </c>
       <c r="E16" s="4">
-        <v>3198.07</v>
-      </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+        <v>5425.8</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1705.79</v>
+      </c>
+      <c r="G16" s="4">
+        <v>242.37</v>
+      </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="3">
@@ -3077,16 +3331,20 @@
         <v>1470.0</v>
       </c>
       <c r="C17" s="4">
-        <v>176310.2</v>
+        <v>295476.33</v>
       </c>
       <c r="D17" s="4">
-        <v>183425.26</v>
+        <v>265590.71</v>
       </c>
       <c r="E17" s="4">
-        <v>7369.1</v>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
+        <v>15245.27</v>
+      </c>
+      <c r="F17" s="4">
+        <v>4292.24</v>
+      </c>
+      <c r="G17" s="4">
+        <v>501.27</v>
+      </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3">
@@ -3096,16 +3354,20 @@
         <v>2451.0</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E18" s="4">
-        <v>21175.89</v>
-      </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+        <v>31895.61</v>
+      </c>
+      <c r="F18" s="4">
+        <v>14138.62</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1752.98</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3">
@@ -3115,16 +3377,20 @@
         <v>3922.0</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E19" s="4">
-        <v>60448.97</v>
-      </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+        <v>90381.42</v>
+      </c>
+      <c r="F19" s="4">
+        <v>40883.97</v>
+      </c>
+      <c r="G19" s="4">
+        <v>4059.83</v>
+      </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="3">
@@ -3134,16 +3400,20 @@
         <v>4903.0</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E20" s="4">
-        <v>116361.62</v>
-      </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
+        <v>156925.56</v>
+      </c>
+      <c r="F20" s="4">
+        <v>58641.39</v>
+      </c>
+      <c r="G20" s="4">
+        <v>6511.26</v>
+      </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="8"/>
@@ -3164,9 +3434,7 @@
       <c r="D23" s="8"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -3178,179 +3446,58 @@
       <c r="D25" s="8"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="B27" s="4">
-        <v>49.0</v>
-      </c>
-      <c r="C27" s="5">
-        <v>11.29</v>
-      </c>
-      <c r="D27" s="5">
-        <v>16.71</v>
-      </c>
-      <c r="E27" s="5">
-        <v>6.63</v>
-      </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="B28" s="4">
-        <v>245.0</v>
-      </c>
-      <c r="C28" s="5">
-        <v>134.72</v>
-      </c>
-      <c r="D28" s="5">
-        <v>271.48</v>
-      </c>
-      <c r="E28" s="5">
-        <v>77.05</v>
-      </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="B29" s="4">
-        <v>490.0</v>
-      </c>
-      <c r="C29" s="5">
-        <v>480.21</v>
-      </c>
-      <c r="D29" s="5">
-        <v>926.24</v>
-      </c>
-      <c r="E29" s="5">
-        <v>217.73</v>
-      </c>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="B30" s="4">
-        <v>980.0</v>
-      </c>
-      <c r="C30" s="5">
-        <v>1901.95</v>
-      </c>
-      <c r="D30" s="5">
-        <v>3471.01</v>
-      </c>
-      <c r="E30" s="5">
-        <v>534.57</v>
-      </c>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="B31" s="4">
-        <v>1470.0</v>
-      </c>
-      <c r="C31" s="5">
-        <v>4453.74</v>
-      </c>
-      <c r="D31" s="5">
-        <v>7945.44</v>
-      </c>
-      <c r="E31" s="5">
-        <v>910.21</v>
-      </c>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="B32" s="4">
-        <v>2451.0</v>
-      </c>
-      <c r="C32" s="5">
-        <v>12329.42</v>
-      </c>
-      <c r="D32" s="5">
-        <v>21427.23</v>
-      </c>
-      <c r="E32" s="5">
-        <v>1658.79</v>
-      </c>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="B33" s="4">
-        <v>3922.0</v>
-      </c>
-      <c r="C33" s="5">
-        <v>32511.23</v>
-      </c>
-      <c r="D33" s="5">
-        <v>60648.2</v>
-      </c>
-      <c r="E33" s="5">
-        <v>3052.8</v>
-      </c>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B34" s="4">
-        <v>4903.0</v>
-      </c>
-      <c r="C34" s="5">
-        <v>49950.18</v>
-      </c>
-      <c r="D34" s="5">
-        <v>88782.28</v>
-      </c>
-      <c r="E34" s="5">
-        <v>4514.55</v>
-      </c>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="8"/>
@@ -3365,179 +3512,58 @@
       <c r="D36" s="8"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="B38" s="4">
-        <v>49.0</v>
-      </c>
-      <c r="C38" s="5">
-        <v>12.95</v>
-      </c>
-      <c r="D38" s="5">
-        <v>30.51</v>
-      </c>
-      <c r="E38" s="5">
-        <v>12.82</v>
-      </c>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="B39" s="4">
-        <v>245.0</v>
-      </c>
-      <c r="C39" s="5">
-        <v>799.27</v>
-      </c>
-      <c r="D39" s="5">
-        <v>827.65</v>
-      </c>
-      <c r="E39" s="5">
-        <v>180.69</v>
-      </c>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="B40" s="4">
-        <v>490.0</v>
-      </c>
-      <c r="C40" s="4">
-        <v>6502.13</v>
-      </c>
-      <c r="D40" s="4">
-        <v>6597.85</v>
-      </c>
-      <c r="E40" s="4">
-        <v>642.96</v>
-      </c>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="B41" s="4">
-        <v>980.0</v>
-      </c>
-      <c r="C41" s="4">
-        <v>51349.88</v>
-      </c>
-      <c r="D41" s="4">
-        <v>57891.29</v>
-      </c>
-      <c r="E41" s="4">
-        <v>3198.07</v>
-      </c>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="B42" s="4">
-        <v>1470.0</v>
-      </c>
-      <c r="C42" s="4">
-        <v>176310.2</v>
-      </c>
-      <c r="D42" s="4">
-        <v>183425.26</v>
-      </c>
-      <c r="E42" s="4">
-        <v>7369.1</v>
-      </c>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="B43" s="4">
-        <v>2451.0</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="4">
-        <v>21175.89</v>
-      </c>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="B44" s="4">
-        <v>3922.0</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="4">
-        <v>60448.97</v>
-      </c>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B45" s="4">
-        <v>4903.0</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="4">
-        <v>116361.62</v>
-      </c>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="8"/>
@@ -3558,9 +3584,7 @@
       <c r="D48" s="8"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -3572,179 +3596,58 @@
       <c r="D50" s="8"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="B52" s="4">
-        <v>49.0</v>
-      </c>
-      <c r="C52" s="5">
-        <v>2.04</v>
-      </c>
-      <c r="D52" s="5">
-        <v>3.38</v>
-      </c>
-      <c r="E52" s="5">
-        <v>1.18</v>
-      </c>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
     </row>
     <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="B53" s="4">
-        <v>245.0</v>
-      </c>
-      <c r="C53" s="5">
-        <v>41.5</v>
-      </c>
-      <c r="D53" s="5">
-        <v>68.55</v>
-      </c>
-      <c r="E53" s="5">
-        <v>16.15</v>
-      </c>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
+      <c r="A53" s="8"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="B54" s="4">
-        <v>490.0</v>
-      </c>
-      <c r="C54" s="5">
-        <v>184.0</v>
-      </c>
-      <c r="D54" s="5">
-        <v>231.097</v>
-      </c>
-      <c r="E54" s="5">
-        <v>43.72</v>
-      </c>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="B55" s="4">
-        <v>980.0</v>
-      </c>
-      <c r="C55" s="5">
-        <v>590.2</v>
-      </c>
-      <c r="D55" s="5">
-        <v>990.164</v>
-      </c>
-      <c r="E55" s="5">
-        <v>103.37</v>
-      </c>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="B56" s="4">
-        <v>1470.0</v>
-      </c>
-      <c r="C56" s="5">
-        <v>1444.3</v>
-      </c>
-      <c r="D56" s="5">
-        <v>1977.63</v>
-      </c>
-      <c r="E56" s="5">
-        <v>182.5</v>
-      </c>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="B57" s="4">
-        <v>2451.0</v>
-      </c>
-      <c r="C57" s="5">
-        <v>3686.54</v>
-      </c>
-      <c r="D57" s="5">
-        <v>5968.38</v>
-      </c>
-      <c r="E57" s="5">
-        <v>338.65</v>
-      </c>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
+      <c r="A57" s="8"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="B58" s="4">
-        <v>3922.0</v>
-      </c>
-      <c r="C58" s="5">
-        <v>10178.65</v>
-      </c>
-      <c r="D58" s="5">
-        <v>15941.24</v>
-      </c>
-      <c r="E58" s="5">
-        <v>668.36</v>
-      </c>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B59" s="4">
-        <v>4903.0</v>
-      </c>
-      <c r="C59" s="5">
-        <v>16736.32</v>
-      </c>
-      <c r="D59" s="5">
-        <v>24646.95</v>
-      </c>
-      <c r="E59" s="5">
-        <v>878.3</v>
-      </c>
-      <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
+      <c r="A59" s="8"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="8"/>
@@ -3759,179 +3662,58 @@
       <c r="D61" s="8"/>
     </row>
     <row r="62" ht="14.25" customHeight="1">
-      <c r="A62" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A62" s="8"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
-      <c r="A63" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="B63" s="4">
-        <v>49.0</v>
-      </c>
-      <c r="C63" s="5">
-        <v>6.43</v>
-      </c>
-      <c r="D63" s="5">
-        <v>7.62</v>
-      </c>
-      <c r="E63" s="5">
-        <v>5.77</v>
-      </c>
-      <c r="F63" s="6"/>
-      <c r="G63" s="6"/>
+      <c r="A63" s="8"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
-      <c r="A64" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="B64" s="4">
-        <v>245.0</v>
-      </c>
-      <c r="C64" s="5">
-        <v>476.3</v>
-      </c>
-      <c r="D64" s="5">
-        <v>520.19</v>
-      </c>
-      <c r="E64" s="5">
-        <v>93.66</v>
-      </c>
-      <c r="F64" s="6"/>
-      <c r="G64" s="6"/>
+      <c r="A64" s="8"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
     </row>
     <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="B65" s="4">
-        <v>490.0</v>
-      </c>
-      <c r="C65" s="4">
-        <v>4376.06</v>
-      </c>
-      <c r="D65" s="4">
-        <v>4927.65</v>
-      </c>
-      <c r="E65" s="4">
-        <v>351.02</v>
-      </c>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
+      <c r="A65" s="8"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="B66" s="4">
-        <v>980.0</v>
-      </c>
-      <c r="C66" s="4">
-        <v>38189.27</v>
-      </c>
-      <c r="D66" s="4">
-        <v>38876.62</v>
-      </c>
-      <c r="E66" s="4">
-        <v>2366.82</v>
-      </c>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
+      <c r="A66" s="8"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="B67" s="4">
-        <v>1470.0</v>
-      </c>
-      <c r="C67" s="4">
-        <v>145345.69</v>
-      </c>
-      <c r="D67" s="4">
-        <v>152477.11</v>
-      </c>
-      <c r="E67" s="4">
-        <v>5426.97</v>
-      </c>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
+      <c r="A67" s="8"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
     </row>
     <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="B68" s="4">
-        <v>2451.0</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="4">
-        <v>16966.43</v>
-      </c>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
+      <c r="A68" s="8"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="B69" s="4">
-        <v>3922.0</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E69" s="4">
-        <v>54118.07</v>
-      </c>
-      <c r="F69" s="9"/>
-      <c r="G69" s="9"/>
+      <c r="A69" s="8"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
-      <c r="A70" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B70" s="4">
-        <v>4903.0</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E70" s="4">
-        <v>104151.47</v>
-      </c>
-      <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
+      <c r="A70" s="8"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
       <c r="A71" s="8"/>
@@ -3958,188 +3740,64 @@
       <c r="D74" s="8"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
+      <c r="A75" s="8"/>
+      <c r="B75" s="8"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A76" s="8"/>
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
     </row>
     <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="B77" s="4">
-        <v>49.0</v>
-      </c>
-      <c r="C77" s="5">
-        <v>7.45</v>
-      </c>
-      <c r="D77" s="5">
-        <v>5.93</v>
-      </c>
-      <c r="E77" s="5">
-        <v>3.17</v>
-      </c>
-      <c r="F77" s="6"/>
-      <c r="G77" s="6"/>
+      <c r="A77" s="8"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="B78" s="4">
-        <v>245.0</v>
-      </c>
-      <c r="C78" s="5">
-        <v>215.79</v>
-      </c>
-      <c r="D78" s="5">
-        <v>104.37</v>
-      </c>
-      <c r="E78" s="5">
-        <v>31.94</v>
-      </c>
-      <c r="F78" s="6"/>
-      <c r="G78" s="6"/>
+      <c r="A78" s="8"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="B79" s="4">
-        <v>490.0</v>
-      </c>
-      <c r="C79" s="5">
-        <v>456036.0</v>
-      </c>
-      <c r="D79" s="5">
-        <v>1042.84</v>
-      </c>
-      <c r="E79" s="5">
-        <v>88.77</v>
-      </c>
-      <c r="F79" s="6"/>
-      <c r="G79" s="6"/>
+      <c r="A79" s="8"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
     </row>
     <row r="80" ht="14.25" customHeight="1">
-      <c r="A80" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="B80" s="4">
-        <v>980.0</v>
-      </c>
-      <c r="C80" s="5">
-        <v>1234.56</v>
-      </c>
-      <c r="D80" s="5">
-        <v>3093.55</v>
-      </c>
-      <c r="E80" s="5">
-        <v>199.55</v>
-      </c>
-      <c r="F80" s="6"/>
-      <c r="G80" s="6"/>
+      <c r="A80" s="8"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
-      <c r="A81" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="B81" s="4">
-        <v>1470.0</v>
-      </c>
-      <c r="C81" s="5">
-        <v>3843.64</v>
-      </c>
-      <c r="D81" s="5">
-        <v>5204.79</v>
-      </c>
-      <c r="E81" s="5">
-        <v>353.86</v>
-      </c>
-      <c r="F81" s="6"/>
-      <c r="G81" s="6"/>
+      <c r="A81" s="8"/>
+      <c r="B81" s="8"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="8"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
-      <c r="A82" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="B82" s="4">
-        <v>2451.0</v>
-      </c>
-      <c r="C82" s="5">
-        <v>8679.57</v>
-      </c>
-      <c r="D82" s="5">
-        <v>13126.63</v>
-      </c>
-      <c r="E82" s="5">
-        <v>634.78</v>
-      </c>
-      <c r="F82" s="6"/>
-      <c r="G82" s="6"/>
+      <c r="A82" s="8"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
     </row>
     <row r="83" ht="14.25" customHeight="1">
-      <c r="A83" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="B83" s="4">
-        <v>3922.0</v>
-      </c>
-      <c r="C83" s="5">
-        <v>21591.45</v>
-      </c>
-      <c r="D83" s="5">
-        <v>34365.41</v>
-      </c>
-      <c r="E83" s="5">
-        <v>1541.28</v>
-      </c>
-      <c r="F83" s="6"/>
-      <c r="G83" s="6"/>
+      <c r="A83" s="8"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
-      <c r="A84" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B84" s="4">
-        <v>4903.0</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E84" s="5">
-        <v>2228.14</v>
-      </c>
-      <c r="F84" s="6"/>
-      <c r="G84" s="6"/>
+      <c r="A84" s="8"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="8"/>
@@ -4154,179 +3812,58 @@
       <c r="D86" s="8"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
-      <c r="A87" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A87" s="8"/>
+      <c r="B87" s="8"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="B88" s="4">
-        <v>49.0</v>
-      </c>
-      <c r="C88" s="5">
-        <v>13.77</v>
-      </c>
-      <c r="D88" s="5">
-        <v>24.95</v>
-      </c>
-      <c r="E88" s="5">
-        <v>17.78</v>
-      </c>
-      <c r="F88" s="6"/>
-      <c r="G88" s="6"/>
+      <c r="A88" s="8"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
     </row>
     <row r="89" ht="14.25" customHeight="1">
-      <c r="A89" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="B89" s="4">
-        <v>245.0</v>
-      </c>
-      <c r="C89" s="5">
-        <v>1299.6</v>
-      </c>
-      <c r="D89" s="5">
-        <v>1646.97</v>
-      </c>
-      <c r="E89" s="5">
-        <v>163.37</v>
-      </c>
-      <c r="F89" s="6"/>
-      <c r="G89" s="6"/>
+      <c r="A89" s="8"/>
+      <c r="B89" s="8"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="8"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
-      <c r="A90" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="B90" s="4">
-        <v>490.0</v>
-      </c>
-      <c r="C90" s="4">
-        <v>898275.0</v>
-      </c>
-      <c r="D90" s="4">
-        <v>12987.7</v>
-      </c>
-      <c r="E90" s="4">
-        <v>570.53</v>
-      </c>
-      <c r="F90" s="9"/>
-      <c r="G90" s="9"/>
+      <c r="A90" s="8"/>
+      <c r="B90" s="8"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
-      <c r="A91" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="B91" s="4">
-        <v>980.0</v>
-      </c>
-      <c r="C91" s="4">
-        <v>88123.87</v>
-      </c>
-      <c r="D91" s="4">
-        <v>79528.31</v>
-      </c>
-      <c r="E91" s="4">
-        <v>5425.8</v>
-      </c>
-      <c r="F91" s="9"/>
-      <c r="G91" s="9"/>
+      <c r="A91" s="8"/>
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
     </row>
     <row r="92" ht="14.25" customHeight="1">
-      <c r="A92" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="B92" s="4">
-        <v>1470.0</v>
-      </c>
-      <c r="C92" s="4">
-        <v>295476.33</v>
-      </c>
-      <c r="D92" s="4">
-        <v>265590.71</v>
-      </c>
-      <c r="E92" s="4">
-        <v>15245.27</v>
-      </c>
-      <c r="F92" s="9"/>
-      <c r="G92" s="9"/>
+      <c r="A92" s="8"/>
+      <c r="B92" s="8"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
-      <c r="A93" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="B93" s="4">
-        <v>2451.0</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="4">
-        <v>31895.61</v>
-      </c>
-      <c r="F93" s="9"/>
-      <c r="G93" s="9"/>
+      <c r="A93" s="8"/>
+      <c r="B93" s="8"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
-      <c r="A94" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="B94" s="4">
-        <v>3922.0</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D94" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E94" s="4">
-        <v>90381.42</v>
-      </c>
-      <c r="F94" s="9"/>
-      <c r="G94" s="9"/>
+      <c r="A94" s="8"/>
+      <c r="B94" s="8"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
     </row>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B95" s="4">
-        <v>4903.0</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E95" s="4">
-        <v>156925.56</v>
-      </c>
-      <c r="F95" s="9"/>
-      <c r="G95" s="9"/>
+      <c r="A95" s="8"/>
+      <c r="B95" s="8"/>
+      <c r="C95" s="8"/>
+      <c r="D95" s="8"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="8"/>
@@ -9763,15 +9300,9 @@
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
-  <tableParts count="8">
-    <tablePart r:id="rId10"/>
-    <tablePart r:id="rId11"/>
-    <tablePart r:id="rId12"/>
-    <tablePart r:id="rId13"/>
-    <tablePart r:id="rId14"/>
-    <tablePart r:id="rId15"/>
-    <tablePart r:id="rId16"/>
-    <tablePart r:id="rId17"/>
+  <tableParts count="2">
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>